<commit_message>
Actualiado con la compra de electrónica
</commit_message>
<xml_diff>
--- a/CW.Potato/Presupuesto/presupuesto.xlsx
+++ b/CW.Potato/Presupuesto/presupuesto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="600" windowWidth="28800" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,42 +18,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Santiago López Pina</author>
-  </authors>
-  <commentList>
-    <comment ref="A11" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Santiago López Pina:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Items para futura compla a corto plazo</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>PRUSA MENDEL.</t>
   </si>
@@ -103,30 +69,12 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Motores</t>
-  </si>
-  <si>
-    <t>http://reprapworld.com/?products_details&amp;products_id=95&amp;cPath=1614</t>
-  </si>
-  <si>
     <t>Rodamientos</t>
   </si>
   <si>
-    <t>http://reprapworld.com/?products_details&amp;products_id=151&amp;cPath=1595_1596</t>
-  </si>
-  <si>
-    <t>Correas T2.5</t>
-  </si>
-  <si>
     <t>http://www.xyzprinters.com/belts/157-prusa-t25-optimized-belt-kit.html</t>
   </si>
   <si>
-    <t>Poleas</t>
-  </si>
-  <si>
-    <t>http://www.redwizard3d.com/products</t>
-  </si>
-  <si>
     <t>Varillas</t>
   </si>
   <si>
@@ -142,14 +90,47 @@
     <t>http://es.rs-online.com/web/p/acero-inoxidable/6614699/</t>
   </si>
   <si>
-    <t>http://www.novoinox.com/varilla-maciza-redonda/2356-varilla-maciza-8mm-aisi-304l-2b-mate.html</t>
+    <t>Sanguinololu</t>
+  </si>
+  <si>
+    <t>http://www.xyzprinters.com/electronics/148-prusa-all-you-need-electronics-kit.html</t>
+  </si>
+  <si>
+    <t>Correas</t>
+  </si>
+  <si>
+    <t>Madera</t>
+  </si>
+  <si>
+    <t>http://www.xyzprinters.com/printbed/90-lower-thickplate.html</t>
+  </si>
+  <si>
+    <t>http://www.xyzprinters.com/metals/154-linear-bearing-kit.html</t>
+  </si>
+  <si>
+    <t>Conector motores</t>
+  </si>
+  <si>
+    <t>http://www.xyzprinters.com/electronics/149-motor-connectors.html</t>
+  </si>
+  <si>
+    <t>Muelles</t>
+  </si>
+  <si>
+    <t>http://www.xyzprinters.com/printbed/94-printbed-springs.html</t>
+  </si>
+  <si>
+    <t>Fuente</t>
+  </si>
+  <si>
+    <t>http://www.xyzprinters.com/electronics/138-420w-pc-power-supply.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -157,40 +138,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -202,21 +156,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -545,11 +493,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -592,6 +540,9 @@
       <c r="A5" s="1">
         <v>40919</v>
       </c>
+      <c r="B5" s="1">
+        <v>40939</v>
+      </c>
       <c r="C5">
         <v>1</v>
       </c>
@@ -685,119 +636,153 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1">
+        <v>40938</v>
+      </c>
+      <c r="B10" s="1">
+        <v>40909</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10">
+        <v>10.42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="11" spans="1:9" ht="15" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3">
-        <v>6</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="A11" s="1">
+        <v>40940</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11">
+        <v>176</v>
+      </c>
+      <c r="F11" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="3">
-        <v>4</v>
-      </c>
-      <c r="F11" s="4" t="s">
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1">
+      <c r="A12" s="1">
+        <v>40941</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1">
+        <v>40942</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1">
+        <v>40943</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4" t="s">
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1">
+        <v>40944</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="3">
-        <v>45</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3">
-        <v>4</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="3">
-        <v>8</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3">
-        <v>1</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="3">
-        <v>22</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="E15">
+        <v>5.5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="3">
-        <v>17</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="A16" s="1">
+        <v>40945</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16">
+        <v>5.6</v>
+      </c>
+      <c r="F16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>40946</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17">
+        <v>28</v>
+      </c>
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="36" spans="4:5">
       <c r="D36" t="s">
@@ -805,16 +790,11 @@
       </c>
       <c r="E36">
         <f>SUM(E5:E35)</f>
-        <v>176.7</v>
+        <v>356.22</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F11" r:id="rId1"/>
-    <hyperlink ref="F12" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Añadidos tornillos que faltaban
</commit_message>
<xml_diff>
--- a/CW.Potato/Presupuesto/presupuesto.xlsx
+++ b/CW.Potato/Presupuesto/presupuesto.xlsx
@@ -18,8 +18,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Santiago López Pina</author>
+  </authors>
+  <commentList>
+    <comment ref="E26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Santiago López Pina:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+No teno precio unitario de cada cosa, en el ticket de todo esto marca 7,60</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>PRUSA MENDEL.</t>
   </si>
@@ -124,13 +158,43 @@
   </si>
   <si>
     <t>http://www.xyzprinters.com/electronics/138-420w-pc-power-supply.html</t>
+  </si>
+  <si>
+    <t>Arandelas M4</t>
+  </si>
+  <si>
+    <t>Arandelas M3</t>
+  </si>
+  <si>
+    <t>Tuercas M4</t>
+  </si>
+  <si>
+    <t>Tuercas M3</t>
+  </si>
+  <si>
+    <t>Tornillos M4x20</t>
+  </si>
+  <si>
+    <t>Tornillos M3x10</t>
+  </si>
+  <si>
+    <t>Tornillos M3x25</t>
+  </si>
+  <si>
+    <t>Tornillos M3x40</t>
+  </si>
+  <si>
+    <t>Prisionero M3</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,13 +202,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -156,15 +255,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -493,11 +605,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -784,17 +896,199 @@
         <v>34</v>
       </c>
     </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>40947</v>
+      </c>
+      <c r="B18" s="1">
+        <v>40947</v>
+      </c>
+      <c r="C18" s="3">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.84440000000000004</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>40947</v>
+      </c>
+      <c r="B19" s="1">
+        <v>40947</v>
+      </c>
+      <c r="C19" s="3">
+        <v>90</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.84440000000000004</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
+        <v>40947</v>
+      </c>
+      <c r="B20" s="1">
+        <v>40947</v>
+      </c>
+      <c r="C20" s="3">
+        <v>4</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.84440000000000004</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>40947</v>
+      </c>
+      <c r="B21" s="1">
+        <v>40947</v>
+      </c>
+      <c r="C21" s="3">
+        <v>90</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.84440000000000004</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
+        <v>40947</v>
+      </c>
+      <c r="B22" s="1">
+        <v>40947</v>
+      </c>
+      <c r="C22" s="3">
+        <v>4</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.84440000000000004</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1">
+        <v>40947</v>
+      </c>
+      <c r="B23" s="1">
+        <v>40947</v>
+      </c>
+      <c r="C23" s="3">
+        <v>30</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.84440000000000004</v>
+      </c>
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1">
+        <v>40947</v>
+      </c>
+      <c r="B24" s="1">
+        <v>40947</v>
+      </c>
+      <c r="C24" s="3">
+        <v>30</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.84440000000000004</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1">
+        <v>40947</v>
+      </c>
+      <c r="B25" s="1">
+        <v>40947</v>
+      </c>
+      <c r="C25" s="3">
+        <v>30</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.84440000000000004</v>
+      </c>
+      <c r="F25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1">
+        <v>40947</v>
+      </c>
+      <c r="B26" s="1">
+        <v>40947</v>
+      </c>
+      <c r="C26" s="3">
+        <v>4</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.84440000000000004</v>
+      </c>
+      <c r="F26" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="36" spans="4:5">
       <c r="D36" t="s">
         <v>15</v>
       </c>
       <c r="E36">
         <f>SUM(E5:E35)</f>
-        <v>356.22</v>
+        <v>363.81960000000009</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Actualizado con Flux y Capton
</commit_message>
<xml_diff>
--- a/CW.Potato/Presupuesto/presupuesto.xlsx
+++ b/CW.Potato/Presupuesto/presupuesto.xlsx
@@ -24,7 +24,7 @@
     <author>Santiago López Pina</author>
   </authors>
   <commentList>
-    <comment ref="E26" authorId="0">
+    <comment ref="E28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>PRUSA MENDEL.</t>
   </si>
@@ -191,6 +191,18 @@
   </si>
   <si>
     <t>http://reprapworld.com/?products_details&amp;products_id=121</t>
+  </si>
+  <si>
+    <t>Capton</t>
+  </si>
+  <si>
+    <t>Flux</t>
+  </si>
+  <si>
+    <t>http://www.dealextreme.com/p/6168</t>
+  </si>
+  <si>
+    <t>http://www.dealextreme.com/p/21361</t>
   </si>
 </sst>
 </file>
@@ -282,12 +294,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -633,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -925,56 +938,50 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1">
-        <v>40942</v>
-      </c>
-      <c r="B18" s="4">
-        <v>40942</v>
-      </c>
-      <c r="C18" s="3">
-        <v>4</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0.84440000000000004</v>
+        <v>40940</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="5">
+        <v>4.1399999999999997</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1">
-        <v>40942</v>
-      </c>
-      <c r="B19" s="4">
-        <v>40942</v>
-      </c>
-      <c r="C19" s="3">
-        <v>90</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="3">
-        <v>0.84440000000000004</v>
+        <v>40940</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="5">
+        <v>2.2000000000000002</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>40942</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="4">
         <v>40942</v>
       </c>
       <c r="C20" s="3">
         <v>4</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E20" s="3">
         <v>0.84440000000000004</v>
@@ -987,14 +994,14 @@
       <c r="A21" s="1">
         <v>40942</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="4">
         <v>40942</v>
       </c>
       <c r="C21" s="3">
         <v>90</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E21" s="3">
         <v>0.84440000000000004</v>
@@ -1014,7 +1021,7 @@
         <v>4</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E22" s="3">
         <v>0.84440000000000004</v>
@@ -1031,10 +1038,10 @@
         <v>40942</v>
       </c>
       <c r="C23" s="3">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E23" s="3">
         <v>0.84440000000000004</v>
@@ -1051,10 +1058,10 @@
         <v>40942</v>
       </c>
       <c r="C24" s="3">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E24" s="3">
         <v>0.84440000000000004</v>
@@ -1074,7 +1081,7 @@
         <v>30</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E25" s="3">
         <v>0.84440000000000004</v>
@@ -1091,10 +1098,10 @@
         <v>40942</v>
       </c>
       <c r="C26" s="3">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E26" s="3">
         <v>0.84440000000000004</v>
@@ -1105,33 +1112,78 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1">
+        <v>40942</v>
+      </c>
+      <c r="B27" s="1">
+        <v>40942</v>
+      </c>
+      <c r="C27" s="3">
+        <v>30</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.84440000000000004</v>
+      </c>
+      <c r="F27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1">
+        <v>40942</v>
+      </c>
+      <c r="B28" s="1">
+        <v>40942</v>
+      </c>
+      <c r="C28" s="3">
+        <v>4</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0.84440000000000004</v>
+      </c>
+      <c r="F28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1">
         <v>40943</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
         <v>44</v>
       </c>
-      <c r="E27">
+      <c r="E29">
         <v>36.5</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="4:5">
-      <c r="D36" t="s">
+    <row r="30" spans="1:6">
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="C31" s="5"/>
+    </row>
+    <row r="38" spans="4:5">
+      <c r="D38" t="s">
         <v>15</v>
       </c>
-      <c r="E36">
-        <f>SUM(E5:E35)</f>
-        <v>400.31960000000009</v>
+      <c r="E38">
+        <f>SUM(E5:E37)</f>
+        <v>406.65960000000007</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Añadido precio de tabla de madera y extrusor
</commit_message>
<xml_diff>
--- a/CW.Potato/Presupuesto/presupuesto.xlsx
+++ b/CW.Potato/Presupuesto/presupuesto.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>PRUSA MENDEL.</t>
   </si>
@@ -203,6 +203,18 @@
   </si>
   <si>
     <t>http://www.dealextreme.com/p/21361</t>
+  </si>
+  <si>
+    <t>Hotend</t>
+  </si>
+  <si>
+    <t>http://www.hotends.com/index.php?route=product/product&amp;product_id=70</t>
+  </si>
+  <si>
+    <t>Maderas aparacio</t>
+  </si>
+  <si>
+    <t>Madera 22,5x22,5</t>
   </si>
 </sst>
 </file>
@@ -277,8 +289,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -302,7 +316,7 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -310,6 +324,7 @@
     <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -317,6 +332,7 @@
     <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -649,7 +665,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -821,6 +837,9 @@
       <c r="A11" s="1">
         <v>40940</v>
       </c>
+      <c r="B11" s="1">
+        <v>40966</v>
+      </c>
       <c r="C11">
         <v>1</v>
       </c>
@@ -838,6 +857,9 @@
       <c r="A12" s="1">
         <v>40940</v>
       </c>
+      <c r="B12" s="1">
+        <v>40966</v>
+      </c>
       <c r="C12">
         <v>1</v>
       </c>
@@ -855,6 +877,9 @@
       <c r="A13" s="1">
         <v>40940</v>
       </c>
+      <c r="B13" s="1">
+        <v>40966</v>
+      </c>
       <c r="C13">
         <v>1</v>
       </c>
@@ -872,6 +897,9 @@
       <c r="A14" s="1">
         <v>40940</v>
       </c>
+      <c r="B14" s="1">
+        <v>40966</v>
+      </c>
       <c r="C14">
         <v>1</v>
       </c>
@@ -889,6 +917,9 @@
       <c r="A15" s="1">
         <v>40940</v>
       </c>
+      <c r="B15" s="1">
+        <v>40966</v>
+      </c>
       <c r="C15">
         <v>1</v>
       </c>
@@ -906,6 +937,9 @@
       <c r="A16" s="1">
         <v>40940</v>
       </c>
+      <c r="B16" s="1">
+        <v>40966</v>
+      </c>
       <c r="C16">
         <v>1</v>
       </c>
@@ -923,6 +957,9 @@
       <c r="A17" s="1">
         <v>40940</v>
       </c>
+      <c r="B17" s="1">
+        <v>40966</v>
+      </c>
       <c r="C17">
         <v>1</v>
       </c>
@@ -1168,10 +1205,38 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="C30" s="5"/>
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="5">
+        <v>50</v>
+      </c>
+      <c r="F30" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="C31" s="5"/>
+      <c r="A31" s="1">
+        <v>41119</v>
+      </c>
+      <c r="B31" s="1">
+        <v>40968</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F31" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="38" spans="4:5">
       <c r="D38" t="s">
@@ -1179,7 +1244,7 @@
       </c>
       <c r="E38">
         <f>SUM(E5:E37)</f>
-        <v>406.65960000000007</v>
+        <v>457.15960000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizado con últimas compras
</commit_message>
<xml_diff>
--- a/CW.Potato/Presupuesto/presupuesto.xlsx
+++ b/CW.Potato/Presupuesto/presupuesto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1460" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <author>Santiago López Pina</author>
   </authors>
   <commentList>
-    <comment ref="E28" authorId="0">
+    <comment ref="E29" authorId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
   <si>
     <t>PRUSA MENDEL.</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Sanguinololu</t>
   </si>
   <si>
-    <t>http://www.xyzprinters.com/electronics/148-prusa-all-you-need-electronics-kit.html</t>
-  </si>
-  <si>
     <t>Correas</t>
   </si>
   <si>
@@ -215,6 +212,69 @@
   </si>
   <si>
     <t>Madera 22,5x22,5</t>
+  </si>
+  <si>
+    <t>Punta soldador 1mm</t>
+  </si>
+  <si>
+    <t>Electrónica Embajadores</t>
+  </si>
+  <si>
+    <t>tacos 7mm</t>
+  </si>
+  <si>
+    <t>Todo a 100</t>
+  </si>
+  <si>
+    <t>Poleas T2.5</t>
+  </si>
+  <si>
+    <t>Espejo</t>
+  </si>
+  <si>
+    <t>http://www.ikea.com/es/es/catalog/products/60074007/?query=60074007#</t>
+  </si>
+  <si>
+    <t>Termometro</t>
+  </si>
+  <si>
+    <t>http://dx.com/p/904435754</t>
+  </si>
+  <si>
+    <t>Muelles 8,5 3cm</t>
+  </si>
+  <si>
+    <t>Tiendas Ros (Ronda de atocha)</t>
+  </si>
+  <si>
+    <t>Rodamientos 608 zz</t>
+  </si>
+  <si>
+    <t>Alberto Valero</t>
+  </si>
+  <si>
+    <t>Sanguinololu pre-soldered</t>
+  </si>
+  <si>
+    <t>http://www.emakershop.com/browse/listing?l=161</t>
+  </si>
+  <si>
+    <t>http://www.reprapbcn.com/catalog/index.php/sls-parts/sls-t2-5-pulley.html</t>
+  </si>
+  <si>
+    <t>Metro de manguera hilo multifilar</t>
+  </si>
+  <si>
+    <t>Tienda electronica.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cd </t>
+  </si>
+  <si>
+    <t>Bridas 4x150</t>
+  </si>
+  <si>
+    <t>Tubo Enrolla cable</t>
   </si>
 </sst>
 </file>
@@ -289,7 +349,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -307,16 +367,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="19"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="24">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -325,6 +394,8 @@
     <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="19" builtinId="8"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -333,6 +404,11 @@
     <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -662,15 +738,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="28.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="70.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -801,7 +877,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -833,24 +909,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1">
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
-        <v>40940</v>
+        <v>40938</v>
       </c>
       <c r="B11" s="1">
-        <v>40966</v>
+        <v>40938</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11">
-        <v>176</v>
+        <v>64</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1">
@@ -864,16 +937,13 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E12">
-        <v>25</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="1">
         <v>40940</v>
       </c>
@@ -884,13 +954,13 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -904,13 +974,13 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E14">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -924,13 +994,13 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E15">
-        <v>5.5</v>
+        <v>24</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -944,13 +1014,13 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E16">
-        <v>5.6</v>
+        <v>5.5</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -964,44 +1034,50 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E17">
-        <v>28</v>
+        <v>5.6</v>
       </c>
       <c r="F17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>40940</v>
       </c>
+      <c r="B18" s="1">
+        <v>40966</v>
+      </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="5">
-        <v>4.1399999999999997</v>
+        <v>32</v>
+      </c>
+      <c r="E18">
+        <v>28</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>40940</v>
       </c>
+      <c r="B19" s="1">
+        <v>40983</v>
+      </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E19" s="5">
-        <v>2.2000000000000002</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="F19" t="s">
         <v>48</v>
@@ -1009,22 +1085,19 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1">
-        <v>40942</v>
-      </c>
-      <c r="B20" s="4">
-        <v>40942</v>
-      </c>
-      <c r="C20" s="3">
-        <v>4</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0.84440000000000004</v>
+        <v>40940</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="5">
+        <v>2.2000000000000002</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1035,10 +1108,10 @@
         <v>40942</v>
       </c>
       <c r="C21" s="3">
-        <v>90</v>
+        <v>4</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E21" s="3">
         <v>0.84440000000000004</v>
@@ -1051,14 +1124,14 @@
       <c r="A22" s="1">
         <v>40942</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="4">
         <v>40942</v>
       </c>
       <c r="C22" s="3">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E22" s="3">
         <v>0.84440000000000004</v>
@@ -1075,10 +1148,10 @@
         <v>40942</v>
       </c>
       <c r="C23" s="3">
-        <v>90</v>
+        <v>4</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E23" s="3">
         <v>0.84440000000000004</v>
@@ -1095,10 +1168,10 @@
         <v>40942</v>
       </c>
       <c r="C24" s="3">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E24" s="3">
         <v>0.84440000000000004</v>
@@ -1115,10 +1188,10 @@
         <v>40942</v>
       </c>
       <c r="C25" s="3">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E25" s="3">
         <v>0.84440000000000004</v>
@@ -1138,7 +1211,7 @@
         <v>30</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E26" s="3">
         <v>0.84440000000000004</v>
@@ -1158,7 +1231,7 @@
         <v>30</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E27" s="3">
         <v>0.84440000000000004</v>
@@ -1175,10 +1248,10 @@
         <v>40942</v>
       </c>
       <c r="C28" s="3">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E28" s="3">
         <v>0.84440000000000004</v>
@@ -1189,67 +1262,281 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
+        <v>40942</v>
+      </c>
+      <c r="B29" s="1">
+        <v>40942</v>
+      </c>
+      <c r="C29" s="3">
+        <v>4</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.84440000000000004</v>
+      </c>
+      <c r="F29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1">
         <v>40943</v>
       </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30">
+        <v>26.72</v>
+      </c>
+      <c r="F30" t="s">
         <v>44</v>
-      </c>
-      <c r="E29">
-        <v>36.5</v>
-      </c>
-      <c r="F29" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="C30" s="3">
-        <v>1</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" s="5">
-        <v>50</v>
-      </c>
-      <c r="F30" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1">
+        <v>40972</v>
+      </c>
+      <c r="C31" s="6">
+        <v>1</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="6">
+        <v>45</v>
+      </c>
+      <c r="F31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1">
         <v>41119</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B32" s="1">
         <v>40968</v>
       </c>
-      <c r="C31" s="3">
-        <v>1</v>
-      </c>
-      <c r="D31" s="3" t="s">
+      <c r="C32" s="6">
+        <v>1</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1">
+        <v>40970</v>
+      </c>
+      <c r="B33" s="1">
+        <v>40970</v>
+      </c>
+      <c r="C33" s="6">
+        <v>1</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="F31" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="4:5">
-      <c r="D38" t="s">
+      <c r="E33" s="6">
+        <v>9.5</v>
+      </c>
+      <c r="F33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="1">
+        <v>40972</v>
+      </c>
+      <c r="B34" s="1">
+        <v>40972</v>
+      </c>
+      <c r="C34" s="6">
+        <v>1</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1">
+        <v>40972</v>
+      </c>
+      <c r="C35" s="6">
+        <v>4</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35">
+        <v>5.7</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="C36" s="6">
+        <v>1</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36">
+        <v>6</v>
+      </c>
+      <c r="F36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="1">
+        <v>40972</v>
+      </c>
+      <c r="C37" s="6">
+        <v>1</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37">
+        <v>20</v>
+      </c>
+      <c r="F37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1">
+        <v>40973</v>
+      </c>
+      <c r="B38" s="1">
+        <v>40973</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="F38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1">
+        <v>40973</v>
+      </c>
+      <c r="B39" s="1">
+        <v>40980</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39">
+        <v>12.5</v>
+      </c>
+      <c r="F39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="1">
+        <v>40984</v>
+      </c>
+      <c r="B40" s="1">
+        <v>40984</v>
+      </c>
+      <c r="C40">
+        <v>10</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40">
+        <v>7.5</v>
+      </c>
+      <c r="F40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1">
+        <v>40987</v>
+      </c>
+      <c r="B41" s="1">
+        <v>40987</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41">
+        <v>1.5</v>
+      </c>
+      <c r="F41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="1">
+        <v>40987</v>
+      </c>
+      <c r="B42" s="1">
+        <v>40987</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42">
+        <v>2.25</v>
+      </c>
+      <c r="F42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="D43" t="s">
         <v>15</v>
       </c>
-      <c r="E38">
-        <f>SUM(E5:E37)</f>
-        <v>457.15960000000007</v>
+      <c r="E43">
+        <f>SUM(E5:E42)</f>
+        <v>510.92960000000011</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F35" r:id="rId1" display="www.reprapbcn.com"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>